<commit_message>
17157 p3 p5 59996,59992,95556,95592,95952
</commit_message>
<xml_diff>
--- a/caipiao.xlsx
+++ b/caipiao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="728">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3005,6 +3005,43 @@
   </si>
   <si>
     <t>389,489,569,689,889,899</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>456789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>239</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2:1
+3:0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>067,156,256,289,388,559,599</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>56789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3456789</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0963258</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>59996,59992,95556,95592,95952</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3139,7 +3176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3273,9 +3310,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3288,7 +3328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3576,8 +3616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="U58" sqref="U58"/>
+    <sheetView topLeftCell="J34" workbookViewId="0">
+      <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6051,26 +6091,50 @@
         <v>718</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="T56" s="8"/>
-      <c r="U56" s="36"/>
+    <row r="56" spans="1:21" s="47" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A56" s="47">
+        <v>17157</v>
+      </c>
+      <c r="B56" s="48">
+        <v>42899</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="57" t="s">
+        <v>722</v>
+      </c>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="H56" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="41" t="s">
+        <v>719</v>
+      </c>
+      <c r="J56" s="41" t="s">
+        <v>720</v>
+      </c>
+      <c r="K56" s="41" t="s">
+        <v>721</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="41"/>
+      <c r="S56" s="41"/>
+      <c r="T56" s="41"/>
+      <c r="U56" s="55" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="57" spans="1:21" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C57" s="8"/>
@@ -6669,10 +6733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y54"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K40" workbookViewId="0">
-      <selection activeCell="X54" sqref="X54"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9258,6 +9322,55 @@
       </c>
       <c r="Y54" s="50"/>
     </row>
+    <row r="55" spans="1:25" s="51" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A55" s="47">
+        <v>17157</v>
+      </c>
+      <c r="B55" s="48">
+        <v>42899</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="D55" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>724</v>
+      </c>
+      <c r="F55" s="50" t="s">
+        <v>725</v>
+      </c>
+      <c r="G55" s="50" t="s">
+        <v>726</v>
+      </c>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="40" t="s">
+        <v>345</v>
+      </c>
+      <c r="L55" s="50" t="s">
+        <v>580</v>
+      </c>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="V55" s="50"/>
+      <c r="W55" s="50"/>
+      <c r="X55" s="41" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y55" s="50"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
17110 dlt 17225 p3p5
</commit_message>
<xml_diff>
--- a/caipiao.xlsx
+++ b/caipiao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="14810" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="14810" windowHeight="7980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P3" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="1301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="1306">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5317,6 +5317,21 @@
   </si>
   <si>
     <t>历史</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>一二五</t>
+  </si>
+  <si>
+    <t>&gt;20 &lt;28</t>
+  </si>
+  <si>
+    <t>7 9 25 32 33,7 9 25 33 34</t>
+  </si>
+  <si>
+    <t>48 6,10</t>
   </si>
 </sst>
 </file>
@@ -11100,7 +11115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K99" workbookViewId="0">
+    <sheetView topLeftCell="A99" workbookViewId="0">
       <selection activeCell="V113" sqref="V113"/>
     </sheetView>
   </sheetViews>
@@ -16362,8 +16377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView topLeftCell="J49" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -19569,7 +19584,7 @@
       <c r="C64" s="82"/>
       <c r="D64" s="82"/>
       <c r="E64" s="82"/>
-      <c r="F64" s="82" t="s">
+      <c r="F64" s="52" t="s">
         <v>1291</v>
       </c>
       <c r="G64" s="82" t="s">
@@ -19581,7 +19596,7 @@
       <c r="I64" s="82" t="s">
         <v>1292</v>
       </c>
-      <c r="J64" s="82" t="s">
+      <c r="J64" s="52" t="s">
         <v>1293</v>
       </c>
       <c r="K64" s="82"/>
@@ -19612,28 +19627,60 @@
       </c>
       <c r="U64" s="82"/>
     </row>
-    <row r="65" spans="3:21" s="54" customFormat="1" ht="13">
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="53"/>
-      <c r="L65" s="53"/>
-      <c r="M65" s="53"/>
-      <c r="N65" s="53"/>
-      <c r="O65" s="53"/>
-      <c r="P65" s="53"/>
-      <c r="Q65" s="53"/>
-      <c r="R65" s="53"/>
-      <c r="S65" s="53"/>
-      <c r="T65" s="53"/>
-      <c r="U65" s="53"/>
-    </row>
-    <row r="66" spans="3:21" s="54" customFormat="1" ht="13">
+    <row r="65" spans="1:21" s="83" customFormat="1" ht="13">
+      <c r="A65" s="83">
+        <v>17110</v>
+      </c>
+      <c r="B65" s="84">
+        <v>42998</v>
+      </c>
+      <c r="C65" s="82"/>
+      <c r="D65" s="82"/>
+      <c r="E65" s="82"/>
+      <c r="F65" s="82" t="s">
+        <v>1301</v>
+      </c>
+      <c r="G65" s="82" t="s">
+        <v>1302</v>
+      </c>
+      <c r="H65" s="105" t="s">
+        <v>789</v>
+      </c>
+      <c r="I65" s="82" t="s">
+        <v>1303</v>
+      </c>
+      <c r="J65" s="82" t="s">
+        <v>1282</v>
+      </c>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="N65" s="94" t="s">
+        <v>793</v>
+      </c>
+      <c r="O65" s="94" t="s">
+        <v>794</v>
+      </c>
+      <c r="P65" s="94" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q65" s="94" t="s">
+        <v>796</v>
+      </c>
+      <c r="R65" s="82" t="s">
+        <v>1238</v>
+      </c>
+      <c r="S65" s="82" t="s">
+        <v>1305</v>
+      </c>
+      <c r="T65" s="82" t="s">
+        <v>1304</v>
+      </c>
+      <c r="U65" s="82"/>
+    </row>
+    <row r="66" spans="1:21" s="54" customFormat="1" ht="13">
       <c r="C66" s="53"/>
       <c r="D66" s="53"/>
       <c r="E66" s="53"/>
@@ -19654,7 +19701,7 @@
       <c r="T66" s="53"/>
       <c r="U66" s="53"/>
     </row>
-    <row r="67" spans="3:21" s="54" customFormat="1" ht="13">
+    <row r="67" spans="1:21" s="54" customFormat="1" ht="13">
       <c r="C67" s="53"/>
       <c r="D67" s="53"/>
       <c r="E67" s="53"/>

</xml_diff>

<commit_message>
17265 p3,p5 17114 dlt
</commit_message>
<xml_diff>
--- a/caipiao.xlsx
+++ b/caipiao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="14810" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="14810" windowHeight="7980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P3" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="1334">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5410,6 +5410,12 @@
   </si>
   <si>
     <t>73447,73443,67446</t>
+  </si>
+  <si>
+    <t>8 21 22 24 31,9 17 18 30 32,11 17 18 32 34,12 16 18 34 35,12 17 18 29 31,14 17 18 29 31</t>
+  </si>
+  <si>
+    <t>5,10</t>
   </si>
 </sst>
 </file>
@@ -11266,7 +11272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K102" workbookViewId="0">
+    <sheetView topLeftCell="K102" workbookViewId="0">
       <selection activeCell="X119" sqref="X119"/>
     </sheetView>
   </sheetViews>
@@ -16630,8 +16636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView topLeftCell="J49" workbookViewId="0">
-      <selection activeCell="T62" sqref="T62"/>
+    <sheetView tabSelected="1" topLeftCell="K49" workbookViewId="0">
+      <selection activeCell="T63" sqref="T63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -19989,24 +19995,52 @@
       <c r="U66" s="82"/>
     </row>
     <row r="67" spans="1:21" s="54" customFormat="1" ht="13">
+      <c r="A67" s="54">
+        <v>17114</v>
+      </c>
+      <c r="B67" s="97">
+        <v>43008</v>
+      </c>
       <c r="C67" s="53"/>
       <c r="D67" s="53"/>
       <c r="E67" s="53"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="53"/>
+      <c r="F67" s="53" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G67" s="105" t="s">
+        <v>1312</v>
+      </c>
+      <c r="H67" s="105" t="s">
+        <v>789</v>
+      </c>
       <c r="I67" s="53"/>
-      <c r="J67" s="53"/>
+      <c r="J67" s="53" t="s">
+        <v>1282</v>
+      </c>
       <c r="K67" s="53"/>
       <c r="L67" s="53"/>
-      <c r="M67" s="53"/>
-      <c r="N67" s="53"/>
-      <c r="O67" s="53"/>
-      <c r="P67" s="53"/>
-      <c r="Q67" s="53"/>
+      <c r="M67" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="N67" s="94" t="s">
+        <v>793</v>
+      </c>
+      <c r="O67" s="94" t="s">
+        <v>794</v>
+      </c>
+      <c r="P67" s="94" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q67" s="94" t="s">
+        <v>796</v>
+      </c>
       <c r="R67" s="53"/>
-      <c r="S67" s="53"/>
-      <c r="T67" s="53"/>
+      <c r="S67" s="53" t="s">
+        <v>1333</v>
+      </c>
+      <c r="T67" s="53" t="s">
+        <v>1332</v>
+      </c>
       <c r="U67" s="53"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JUST NEED A LITTLE LUCK.
</commit_message>
<xml_diff>
--- a/caipiao.xlsx
+++ b/caipiao.xlsx
@@ -11,12 +11,12 @@
     <sheet name="P5" sheetId="2" r:id="rId2"/>
     <sheet name="DLT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="1406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1412">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5638,12 +5638,32 @@
   <si>
     <t>11 18 19 28 30,11 18 20 28 29</t>
   </si>
+  <si>
+    <t>12 20 21 23 34,12 21 23 24 33,12 21 23 24 34,13 19 21 22 34,13 19 21 22 35,13 21 22 24 34</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>5 20 22 29 30,5 20 22 34 35,5 21 22 24 34,5 21 22 24 35
+,5 21 22 29 31,5 21 26 27 29,5 21 27 29 30</t>
+  </si>
+  <si>
+    <t>21,24</t>
+  </si>
+  <si>
+    <t>22-27</t>
+  </si>
+  <si>
+    <t>8 21 22 24 31,8 21 22 24 32,8 21 22 24 33,8 21 22 24 34,
+8 21 22 24 35,9 21 22 24 33,10 21 22 24 33,11 21 22 24 33,13 21 22 24 35</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5772,6 +5792,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -5851,7 +5878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6099,6 +6126,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17373,8 +17408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="112" workbookViewId="0">
-      <selection activeCell="P79" sqref="P79"/>
+    <sheetView tabSelected="1" topLeftCell="M76" zoomScale="112" workbookViewId="0">
+      <selection activeCell="T88" sqref="T87:T88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -21377,72 +21412,155 @@
       <c r="U79" s="44"/>
     </row>
     <row r="80" spans="1:21" s="43" customFormat="1">
-      <c r="B80" s="107"/>
+      <c r="A80" s="43">
+        <v>17136</v>
+      </c>
+      <c r="B80" s="108">
+        <v>43059</v>
+      </c>
       <c r="C80" s="44"/>
       <c r="D80" s="44"/>
       <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
+      <c r="F80" s="44" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G80" s="44" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H80" s="44" t="s">
+        <v>789</v>
+      </c>
       <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
+      <c r="J80" s="44" t="s">
+        <v>1282</v>
+      </c>
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
-      <c r="O80" s="44"/>
-      <c r="P80" s="44"/>
-      <c r="Q80" s="44"/>
+      <c r="M80" s="114" t="s">
+        <v>792</v>
+      </c>
+      <c r="N80" s="114" t="s">
+        <v>793</v>
+      </c>
+      <c r="O80" s="114" t="s">
+        <v>794</v>
+      </c>
+      <c r="P80" s="114" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q80" s="114" t="s">
+        <v>796</v>
+      </c>
       <c r="R80" s="44"/>
-      <c r="S80" s="44"/>
-      <c r="T80" s="44"/>
+      <c r="S80" s="44" t="s">
+        <v>1336</v>
+      </c>
+      <c r="T80" s="44" t="s">
+        <v>1406</v>
+      </c>
       <c r="U80" s="44"/>
     </row>
-    <row r="81" spans="2:21" s="43" customFormat="1">
-      <c r="B81" s="107"/>
-      <c r="C81" s="44"/>
-      <c r="D81" s="44"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="44"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="44"/>
-      <c r="M81" s="44"/>
-      <c r="N81" s="44"/>
-      <c r="O81" s="44"/>
-      <c r="P81" s="44"/>
-      <c r="Q81" s="44"/>
-      <c r="R81" s="44"/>
-      <c r="S81" s="44"/>
-      <c r="T81" s="44"/>
-      <c r="U81" s="44"/>
-    </row>
-    <row r="82" spans="2:21" s="43" customFormat="1">
-      <c r="B82" s="107"/>
+    <row r="81" spans="1:21" s="117" customFormat="1" ht="29">
+      <c r="A81" s="117">
+        <v>17137</v>
+      </c>
+      <c r="B81" s="118">
+        <v>43060</v>
+      </c>
+      <c r="C81" s="102"/>
+      <c r="D81" s="102"/>
+      <c r="E81" s="102"/>
+      <c r="F81" s="102" t="s">
+        <v>1407</v>
+      </c>
+      <c r="G81" s="102" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H81" s="102" t="s">
+        <v>789</v>
+      </c>
+      <c r="I81" s="102"/>
+      <c r="J81" s="121" t="s">
+        <v>1282</v>
+      </c>
+      <c r="K81" s="102"/>
+      <c r="L81" s="102"/>
+      <c r="M81" s="119" t="s">
+        <v>792</v>
+      </c>
+      <c r="N81" s="119" t="s">
+        <v>793</v>
+      </c>
+      <c r="O81" s="119" t="s">
+        <v>794</v>
+      </c>
+      <c r="P81" s="119" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q81" s="119" t="s">
+        <v>796</v>
+      </c>
+      <c r="R81" s="102"/>
+      <c r="S81" s="102" t="s">
+        <v>1359</v>
+      </c>
+      <c r="T81" s="120" t="s">
+        <v>1408</v>
+      </c>
+      <c r="U81" s="102"/>
+    </row>
+    <row r="82" spans="1:21" s="43" customFormat="1" ht="29">
+      <c r="A82" s="43">
+        <v>17138</v>
+      </c>
+      <c r="B82" s="122">
+        <v>43064</v>
+      </c>
       <c r="C82" s="44"/>
       <c r="D82" s="44"/>
       <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="44"/>
+      <c r="F82" s="44" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G82" s="44" t="s">
+        <v>1373</v>
+      </c>
+      <c r="H82" s="44" t="s">
+        <v>789</v>
+      </c>
+      <c r="I82" s="44" t="s">
+        <v>1410</v>
+      </c>
+      <c r="J82" s="44" t="s">
+        <v>1282</v>
+      </c>
       <c r="K82" s="44"/>
-      <c r="L82" s="44"/>
-      <c r="M82" s="44"/>
-      <c r="N82" s="44"/>
-      <c r="O82" s="44"/>
-      <c r="P82" s="44"/>
-      <c r="Q82" s="44"/>
+      <c r="L82" s="44" t="s">
+        <v>1409</v>
+      </c>
+      <c r="M82" s="114" t="s">
+        <v>792</v>
+      </c>
+      <c r="N82" s="114" t="s">
+        <v>793</v>
+      </c>
+      <c r="O82" s="114" t="s">
+        <v>794</v>
+      </c>
+      <c r="P82" s="114" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q82" s="114" t="s">
+        <v>796</v>
+      </c>
       <c r="R82" s="44"/>
       <c r="S82" s="44"/>
-      <c r="T82" s="44"/>
+      <c r="T82" s="116" t="s">
+        <v>1411</v>
+      </c>
       <c r="U82" s="44"/>
     </row>
-    <row r="83" spans="2:21" s="43" customFormat="1">
+    <row r="83" spans="1:21" s="43" customFormat="1">
       <c r="B83" s="107"/>
       <c r="C83" s="44"/>
       <c r="D83" s="44"/>
@@ -21464,7 +21582,7 @@
       <c r="T83" s="44"/>
       <c r="U83" s="44"/>
     </row>
-    <row r="84" spans="2:21" s="43" customFormat="1">
+    <row r="84" spans="1:21" s="43" customFormat="1">
       <c r="B84" s="107"/>
       <c r="C84" s="44"/>
       <c r="D84" s="44"/>

</xml_diff>